<commit_message>
feat: add visualization for language-specific features properties
</commit_message>
<xml_diff>
--- a/active_features/meta-llama/Llama-3.2-1B/EleutherAI/sae-Llama-3.2-1B-131k/count/result.xlsx
+++ b/active_features/meta-llama/Llama-3.2-1B/EleutherAI/sae-Llama-3.2-1B-131k/count/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lyzander Andrylie\Documents\(1) Ilmu Komputer\TA\code\TA\active_features\meta-llama\Llama-3.2-1B\EleutherAI\sae-Llama-3.2-1B-131k\count\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D423A9E-4746-4B36-BA05-A59FB0731F1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA5DA81-A1AE-428D-A8FA-987D16290E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,21 +23,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="148">
   <si>
-    <t>layer</t>
-  </si>
-  <si>
-    <t>lang</t>
-  </si>
-  <si>
-    <t>feature_id</t>
-  </si>
-  <si>
-    <t>interpretation</t>
-  </si>
-  <si>
-    <t>tokens</t>
-  </si>
-  <si>
     <t>model.layers.0.mlp</t>
   </si>
   <si>
@@ -465,6 +450,21 @@
   </si>
   <si>
     <t>"Suffixes such as \"ı\", \"lar\", \"ler\", \"lık\", \"lık\", \"im\", \"in\", \"isi\", \"lığı\", \"ları\", \"leri\", \"ını\", \"udur\", \"ildi\", \"ım\", \"isi\", \"arı\", \"alı\", \"isi\", \"lık\"</t>
+  </si>
+  <si>
+    <t>Layer</t>
+  </si>
+  <si>
+    <t>Lang</t>
+  </si>
+  <si>
+    <t>Feature ID</t>
+  </si>
+  <si>
+    <t>Interpretation</t>
+  </si>
+  <si>
+    <t>Tokens</t>
   </si>
 </sst>
 </file>
@@ -854,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,189 +869,189 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>145</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>3</v>
+        <v>146</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>4</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5">
         <v>93066</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5">
         <v>128132</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5">
         <v>14207</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="C5" s="5">
         <v>34138</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="C6" s="5">
         <v>12333</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C7" s="5">
         <v>123973</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C8" s="5">
         <v>19293</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="C9" s="5">
         <v>37895</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C10" s="5">
         <v>5889</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="138" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C11" s="5">
         <v>67343</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1065,7 +1065,7 @@
   <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1079,1039 +1079,1039 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>145</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>3</v>
+        <v>146</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>4</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C2" s="5">
         <v>123218</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C3" s="5">
         <v>93066</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5">
         <v>64723</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C5" s="5">
         <v>32578</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C6" s="5">
         <v>84692</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C7" s="5">
         <v>14207</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C8" s="5">
         <v>56064</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C9" s="5">
         <v>100192</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C10" s="5">
         <v>105874</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C11" s="5">
         <v>98476</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C12" s="5">
         <v>120200</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C13" s="5">
         <v>4518</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C14" s="5">
         <v>48343</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="C15" s="5">
         <v>12333</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="C16" s="5">
         <v>30265</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C17" s="5">
         <v>31366</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C18" s="5">
         <v>49501</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C19" s="5">
         <v>121507</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C20" s="5">
         <v>68498</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C21" s="5">
         <v>70835</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C22" s="5">
         <v>123973</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C23" s="5">
         <v>79729</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C24" s="5">
         <v>109317</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C25" s="5">
         <v>9083</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C26" s="5">
         <v>77250</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C27" s="5">
         <v>59767</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C28" s="5">
         <v>41383</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C29" s="5">
         <v>43549</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C30" s="5">
         <v>44371</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C31" s="5">
         <v>56594</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C32" s="5">
         <v>52975</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C33" s="5">
         <v>27401</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C34" s="5">
         <v>52681</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C35" s="5">
         <v>63085</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C36" s="5">
         <v>102511</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="138" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C37" s="5">
         <v>8452</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C38" s="5">
         <v>74675</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="C39" s="5">
         <v>37895</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C40" s="5">
         <v>16648</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C41" s="5">
         <v>13954</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C42" s="5">
         <v>31110</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C43" s="5">
         <v>48228</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C44" s="5">
         <v>91108</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C45" s="5">
         <v>29244</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C46" s="5">
         <v>40052</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C47" s="5">
         <v>97322</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C48" s="5">
         <v>115738</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="C49" s="5">
         <v>53088</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C50" s="5">
         <v>40808</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C51" s="5">
         <v>14651</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C52" s="5">
         <v>312</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C53" s="5">
         <v>27401</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C54" s="5">
         <v>108954</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="C55" s="5">
         <v>44860</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C56" s="5">
         <v>5889</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="138" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C57" s="5">
         <v>17109</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C58" s="5">
         <v>75403</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C59" s="5">
         <v>130833</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C60" s="5">
         <v>56964</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="138" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C61" s="5">
         <v>66481</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: add highlight to the interpretations
</commit_message>
<xml_diff>
--- a/active_features/meta-llama/Llama-3.2-1B/EleutherAI/sae-Llama-3.2-1B-131k/count/result.xlsx
+++ b/active_features/meta-llama/Llama-3.2-1B/EleutherAI/sae-Llama-3.2-1B-131k/count/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lyzander Andrylie\Documents\(1) Ilmu Komputer\TA\code\TA\active_features\meta-llama\Llama-3.2-1B\EleutherAI\sae-Llama-3.2-1B-131k\count\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA5DA81-A1AE-428D-A8FA-987D16290E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEA66B6-4F08-4140-ACE2-7C143CD19489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="163">
   <si>
     <t>model.layers.0.mlp</t>
   </si>
@@ -59,15 +59,9 @@
     <t>"Highly frequent activations on punctuation marks, especially commas and spaces, often at the start of sentences or clauses, and across multiple languages, indicating a focus on structural or delimiting tokens in multilingual text."</t>
   </si>
   <si>
-    <t>"The highlighted tokens are primarily function words (such as articles, conjunctions, prepositions, and auxiliary verbs) and common noun phrases that serve as structural anchors in sentences. These tokens often mark the boundaries of clauses, introduce or connect ideas, and are essential for grammatical cohesion and meaning flow in both narrative and informational contexts."</t>
-  </si>
-  <si>
     <t>"The highlighted tokens are often function words, conjunctions, prepositions, or common short phrases that serve as syntactic connectors or modifiers, as well as inflectional or derivational morphemes in various languages. These tokens are crucial for sentence structure, meaning transitions, and grammatical relationships across diverse linguistic contexts."</t>
   </si>
   <si>
-    <t>"The highlighted text segments are typically multi-word phrases or clauses that convey specific actions, states, or relationships, often providing key contextual or descriptive information within a sentence. These segments frequently include verbs, objects, and modifiers, forming meaningful units that contribute to the overall narrative or informational structure of the text."</t>
-  </si>
-  <si>
     <t>"The highlighted tokens are predominantly suffixes, prefixes, or inflectional endings in Bulgarian (and occasionally other languages), marking grammatical features such as tense, number, gender, case, or aspect, as well as forming participles, adjectives, and nouns. These morphemes are essential for word formation and grammatical agreement in the language."</t>
   </si>
   <si>
@@ -83,9 +77,6 @@
     <t>"The highlighted tokens frequently correspond to structural elements in formal or factual writing, such as numbers, dates, conjunctions, prepositions, punctuation, and proper nouns, which are often used to organize, enumerate, or specify information in lists, references, or descriptive passages."</t>
   </si>
   <si>
-    <t>"The text contains a wide variety of conversational and narrative fragments, including idiomatic expressions, filler words, discourse markers, and references to people, places, and actions. There is a frequent use of pronouns, conjunctions, and auxiliary verbs, as well as sequences that reflect spoken language patterns such as repetitions, hesitations, and clarifications. Many segments highlight the structure of dialogue, question-answer formats, and descriptive or explanatory statements, often focusing on actions, states, or relationships between entities."</t>
-  </si>
-  <si>
     <t xml:space="preserve"> has,  been,  the, ,, ,,  and,  for, ,,  as,  well,  as,  co,  for,  all,  of</t>
   </si>
   <si>
@@ -170,9 +161,6 @@
     <t>"The highlighted tokens are predominantly prefixes, roots, or short morphemes within words, often marking the beginning or core of nouns, verbs, or adjectives across multiple languages. These segments frequently correspond to meaningful subword units, such as roots, affixes, or syllables, and are often found in proper names, technical terms, or compound words. The pattern reflects a focus on linguistically significant subword structures that contribute to word formation and meaning."</t>
   </si>
   <si>
-    <t>"The highlighted tokens are primarily German morphemes, word stems, or inflections, often marking noun or verb endings, compound word parts, or grammatical function words. Many are common in German-language text, including noun endings (-en, -heit, -keit, -ung), verb forms (-iert, -te, -en), and connecting words (und, von, in, der, die, das, eine). There is also frequent activation on recurring roots in compound nouns and on inflectional suffixes, reflecting the morphological structure of German."</t>
-  </si>
-  <si>
     <t>"The highlighted tokens are often function words, affixes, or short morphemes in various languages, including prepositions, conjunctions, pronouns, and grammatical particles, as well as some high-activation non-standard or corrupted characters. These tokens are typically important for sentence structure, meaning, or language identification."</t>
   </si>
   <si>
@@ -188,102 +176,45 @@
     <t>"The highlighted tokens are often morphemes, word stems, or affixes from various languages, especially Spanish, marking grammatical or semantic units such as verb endings, noun forms, or prepositions, and sometimes appear in named entities or set phrases."</t>
   </si>
   <si>
-    <t>"The highlighted tokens are primarily short morphemes, prefixes, or function words in Slavic and related languages, often marking grammatical relationships, word formation, or serving as connectors within or between words and phrases."</t>
-  </si>
-  <si>
     <t>"The highlighted tokens are predominantly suffixes, inflections, or short morphemes in Bulgarian (and some other languages), such as grammatical endings for tense, case, gender, number, or diminutives, as well as common function words and particles. These elements are crucial for the grammatical structure and meaning of words and sentences."</t>
   </si>
   <si>
-    <t>"The highlighted tokens are primarily German (and some Russian) morphemes, word stems, and inflectional endings, often marking grammatical features such as case, number, tense, or forming compound nouns and verbs. Many are parts of longer words or compounds, reflecting the agglutinative and inflectional nature of German, and are often found at the beginning, middle, or end of words."</t>
-  </si>
-  <si>
     <t>"The highlighted tokens are characteristic morphemes, suffixes, or letter clusters commonly found in Romanian and related Eastern European place names, river names, and surnames, often marking grammatical or regional features."</t>
   </si>
   <si>
-    <t>"The highlighted tokens are predominantly morphemes, roots, prefixes, suffixes, or short function words within Russian, Bulgarian, and related Slavic texts. These segments often mark grammatical features, word formation, or serve as connectors, and are frequently found at the beginning, middle, or end of words, reflecting the agglutinative and inflectional nature of these languages."</t>
-  </si>
-  <si>
     <t>"The highlighted tokens are morphemes or syllables at word boundaries across multiple languages, often marking inflections, derivations, or meaningful subword units. These include suffixes, prefixes, or roots that contribute to the grammatical or semantic structure of words."</t>
   </si>
   <si>
     <t>"The highlighted tokens are primarily morphemes, syllables, or short word fragments from multiple languages, especially Thai, Russian, and Bulgarian, often marking the start or core of content words such as nouns, verbs, or adjectives. These fragments frequently appear at the beginning or within important words, indicating their role in word formation and semantic content across diverse scripts and languages."</t>
   </si>
   <si>
-    <t>"The highlighted tokens are primarily German function words, verb forms, noun and adjective endings, and common prefixes or suffixes, often marking grammatical relationships, tense, plurality, or case, as well as frequent collocations and set phrases. These tokens are essential for sentence structure and meaning in German text."</t>
-  </si>
-  <si>
-    <t>"The highlighted tokens are primarily morphemes, word stems, suffixes, and grammatical endings in Russian (and some in English), often marking case, number, tense, or forming nouns, adjectives, and verbs. There is a focus on functional elements that contribute to word formation, inflection, and syntactic structure, as well as on common connective words and phrase boundaries."</t>
-  </si>
-  <si>
-    <t>"The highlighted tokens are primarily function words, verb forms, noun and adjective endings, and common collocations in German sentences, often marking grammatical structure, tense, or case, as well as frequent phrase boundaries and connectors. These tokens are crucial for sentence construction and meaning in German text."</t>
-  </si>
-  <si>
     <t>"The highlighted tokens are predominantly prefixes, suffixes, or stems within Portuguese words, often marking verb conjugations, noun/adjective forms, or common morphemes. These segments frequently appear at the start or end of words, reflecting morphological structure and inflectional patterns in the language."</t>
   </si>
   <si>
-    <t>"The highlighted tokens are predominantly Russian word stems, prefixes, and suffixes that form the core of verbs, nouns, and adjectives, often marking grammatical or semantic roles such as actions, objects, or qualities. These morphemes are crucial for word formation and meaning in Russian, frequently appearing at the beginning or within words to indicate tense, aspect, subject, or object, and are central to the structure and interpretation of Russian sentences."</t>
-  </si>
-  <si>
     <t>"The highlighted tokens are predominantly proper nouns, especially names of people, places, and media titles, often appearing in multiple languages and scripts. These tokens frequently occur in contexts involving legal, journalistic, or entertainment references, and are often accompanied by titles, roles, or institutional affiliations."</t>
   </si>
   <si>
     <t>"The highlighted tokens are primarily function words, pronouns, conjunctions, prepositions, and common verb forms in Bulgarian (and some in other languages), as well as frequent morphemes and endings. These elements are essential for sentence structure, grammatical relationships, and meaning, often marking tense, negation, possession, or subordination. The activations focus on the connective tissue of language that enables coherent and contextually appropriate communication."</t>
   </si>
   <si>
-    <t>"The highlighted spans are predominantly German multi-word expressions, noun or verb phrases, and compound words, often marking grammatical constructs, inflections, or idiomatic units. Many are functionally important for sentence structure, such as verb-final clauses, participial forms, or noun compounds, and frequently include suffixes or prefixes that signal tense, plurality, or case. These patterns reflect the morphological richness and syntactic dependencies characteristic of German text."</t>
-  </si>
-  <si>
-    <t>"The highlighted tokens are predominantly proper nouns, technical terms, and named entities—such as personal names, place names, and institutional or scientific terms—often in multiple languages. These tokens frequently appear in contexts involving formal identification, attribution, or description of people, locations, organizations, or specialized concepts."</t>
-  </si>
-  <si>
     <t>"The highlighted tokens are predominantly short function words, prefixes, or single letters from various languages, often marking grammatical relationships, verb forms, or serving as conjunctions and prepositions. These tokens are crucial for sentence structure and meaning, especially in morphologically rich or agglutinative languages."</t>
   </si>
   <si>
-    <t>"The highlighted tokens are predominantly German morphemes, word stems, and grammatical endings, often marking inflections, compounds, or function words. These tokens frequently appear at the boundaries of words or phrases, indicating their importance for understanding German syntax, morphology, and sentence structure."</t>
-  </si>
-  <si>
-    <t>"The highlighted tokens are primarily German function words, verb forms, pronouns, and common noun or adjective suffixes, especially those marking person, tense, or plurality. There is a strong focus on grammatical structures, such as verb conjugations, modal verbs, and case endings, as well as on frequently used collocations and phrasal patterns in German sentences."</t>
-  </si>
-  <si>
     <t>"The text contains frequent use of Hindi conjuncts and half-letters, especially the \"्\" (virama) and combinations with \"व\", \"र\", \"य\", and other consonants, which are characteristic of Hindi morphology and word formation, particularly in formal or technical contexts."</t>
   </si>
   <si>
     <t>"The highlighted tokens are predominantly Korean noun and suffix forms, often ending with \"함\", \"것\", \"음\", \"법\", \"형\", \"율\", \"량\", \"군\", \"객\", \"면\", \"성\", \"전\", \"편\", \"심\", \"득\", \"상\", \"시간\", and similar morphemes. These tokens typically denote abstract concepts, objects, people, or states, and are frequently used as nominalizers or to form compound nouns, reflecting a pattern of marking key semantic units or grammatical roles in Korean text."</t>
   </si>
   <si>
-    <t>"The highlighted tokens are predominantly Russian morphemes, words, or short phrases that serve as key semantic or syntactic units within sentences. They include verb roots, noun endings, pronouns, conjunctions, and common collocations, often marking the core meaning, grammatical structure, or transitions in the text. The activations focus on elements that define actions, states, relationships, or important contextual information, reflecting the building blocks of Russian sentence construction and meaning."</t>
-  </si>
-  <si>
-    <t>"The highlighted tokens are primarily Russian morphemes, roots, and affixes that form the core semantic or grammatical structure of words, often marking verbs, nouns, or adjectives, and are crucial for conveying meaning, tense, aspect, or function within the sentence."</t>
-  </si>
-  <si>
     <t>"The highlighted tokens are predominantly suffixes or stems in Bulgarian that form adjectives, nouns, or participles, often indicating grammatical features such as gender, number, or case, and are especially common in forming complex or compound words. These morphemes frequently appear at the end of words and are central to word formation and inflection in the language."</t>
   </si>
   <si>
     <t>"Suffixes and endings in Hindi, such as े, ं, ा, ी, ै, ों, and ें, are frequently activated, reflecting their grammatical role in verb conjugation, noun/adjective inflection, and pluralization. These endings are crucial for indicating tense, number, gender, and case in Hindi sentences."</t>
   </si>
   <si>
-    <t>"The highlighted tokens are predominantly Russian morphemes, roots, or affixes that form the core semantic or grammatical structure of words, often marking verbs, adjectives, or nouns. These segments frequently appear at the beginning or end of words and are essential for conveying meaning, tense, aspect, or other grammatical features in Russian. The activations focus on these meaningful subword units that are central to word formation and comprehension in the language."</t>
-  </si>
-  <si>
-    <t>"The highlighted tokens are primarily Russian morphemes, function words, and endings that mark grammatical relationships, verb conjugations, noun/adjective declensions, and common syntactic connectors. These tokens are crucial for sentence structure, tense, case, agreement, and linking clauses, reflecting the morphological richness and syntactic dependencies of Russian language."</t>
-  </si>
-  <si>
     <t>"The text highlights the importance of common Bulgarian prefixes such as \"из\", \"под\", \"раз\", \"съ\", \"при\", and others, which frequently appear at the beginning of words to form verbs, nouns, or adjectives. These prefixes are key morphological markers that modify the meaning of root words and are highly salient in the structure and semantics of Bulgarian language."</t>
   </si>
   <si>
-    <t>"The highlighted tokens are primarily morphemes, roots, prefixes, and suffixes within Russian words, often marking word formation, inflection, or derivation. These segments frequently correspond to meaningful subword units that contribute to the grammatical or semantic structure of the word, such as case endings, diminutives, verb aspects, or noun/adjective formation."</t>
-  </si>
-  <si>
-    <t>"The highlighted tokens are predominantly Russian (and some other Slavic) word endings, suffixes, and inflections that indicate grammatical case, number, gender, verb tense, or derivational morphology. These endings are crucial for understanding syntactic roles and semantic relationships in the text, as well as for identifying noun, adjective, and verb forms."</t>
-  </si>
-  <si>
-    <t>"The highlighted tokens are predominantly Russian morphological suffixes, prepositions, conjunctions, and noun/adjective endings that indicate grammatical relationships, case, number, gender, and aspect. These elements are essential for syntactic structure and meaning in Russian, often marking possession, agency, time, and other core grammatical functions."</t>
-  </si>
-  <si>
-    <t>"The important tokens are predominantly Russian morphemes, roots, and affixes that form the core semantic or grammatical structure of words, often marking noun, verb, or adjective stems, as well as common derivational and inflectional endings. These tokens frequently appear at the beginning or within the main body of words, highlighting the morphological building blocks essential for meaning and word formation in Russian text."</t>
-  </si>
-  <si>
     <t>"The highlighted tokens are primarily Spanish morphemes, suffixes, and function words, including endings for adjectives, nouns, and adverbs, as well as conjunctions, prepositions, and common connectors. There is also emphasis on punctuation and proper nouns, reflecting structural and grammatical elements essential for sentence construction and meaning in Spanish text."</t>
   </si>
   <si>
@@ -293,30 +224,12 @@
     <t>"The highlighted tokens are predominantly Bulgarian morphemes, suffixes, and inflections that mark grammatical features such as tense, number, gender, case, and aspect, as well as common function words and short stems. These elements are crucial for the syntactic and semantic structure of Bulgarian sentences, often appearing at the ends of words or as short connecting words, reflecting the language's rich inflectional morphology."</t>
   </si>
   <si>
-    <t>"The highlighted tokens are predominantly German suffixes and word endings that form nouns, adjectives, and participles, often indicating grammatical features such as case, number, gender, or degree, as well as forming compound words and inflections."</t>
-  </si>
-  <si>
     <t>"Single uppercase letters or digraphs, often at the start of a word or name, are highlighted across multiple languages and scripts, frequently marking proper nouns, initials, or abbreviations."</t>
   </si>
   <si>
     <t>"The highlighted tokens are common Hindi suffixes and vowel diacritics, such as \"ा\", \"ी\", \"े\", \"ै\", and \"ें\", which are essential for inflection, tense, plurality, and grammatical agreement in Hindi words. These suffixes frequently appear at the end of verbs, nouns, and adjectives, marking grammatical features and contributing to the overall meaning and structure of sentences."</t>
   </si>
   <si>
-    <t>"The highlighted tokens are predominantly Russian morphemes, roots, and affixes that form the core semantic or grammatical structure of words. These include verb and noun roots, derivational and inflectional suffixes, and key word segments that contribute to meaning, tense, aspect, or case. The pattern reflects a focus on the internal morphological structure of Russian words, emphasizing the parts that carry essential lexical or grammatical information."</t>
-  </si>
-  <si>
-    <t>"The highlighted tokens are primarily German morphemes, function words, and common suffixes or inflections, as well as high-frequency connectors and pronouns. These include verb and noun endings, conjunctions, prepositions, and pronouns, which are essential for sentence structure and meaning in German text. The activations also emphasize recurring grammatical patterns, such as subordinate clause markers, verb conjugations, and noun/adjective endings, reflecting the importance of syntactic and morphological elements in German language processing."</t>
-  </si>
-  <si>
-    <t>"The highlighted tokens are predominantly German morphemes, function words, and common suffixes or inflections, often marking verb forms, noun endings, or grammatical particles. These tokens frequently appear at the boundaries of words or as part of compound constructions, reflecting the morphological richness and syntactic structure of German text."</t>
-  </si>
-  <si>
-    <t>"The highlighted tokens are predominantly German function words, inflectional endings, and common noun or adjective suffixes, reflecting grammatical structure such as articles, pronouns, prepositions, conjunctions, and case or number markers essential for sentence construction and meaning."</t>
-  </si>
-  <si>
-    <t>"The highlighted tokens are primarily Russian morphemes, roots, and affixes that form the semantic and grammatical core of words, often marking key concepts, actions, or relationships within sentences. These include noun, verb, and adjective roots, as well as frequent derivational and inflectional suffixes, reflecting the morphological structure and meaning-bearing elements of the language."</t>
-  </si>
-  <si>
     <t>"The highlighted tokens are primarily Thai morphemes, syllables, or short words that serve as key semantic or grammatical units within sentences. These tokens often mark the beginnings or important parts of compound words, function words, or content words, and are frequently found at the start of phrases, within compound constructions, or as part of inflectional or derivational morphology. The pattern reflects the segmentation of Thai text into meaningful subword units that are crucial for understanding sentence structure and meaning."</t>
   </si>
   <si>
@@ -465,6 +378,2167 @@
   </si>
   <si>
     <t>Tokens</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"Highly frequent activations on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>punctuation marks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, especially </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>commas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>spaces</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>often at the start of sentences or clauses</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, and across multiple languages, indicating </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">a focus on structural or delimiting tokens </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>in multilingual text."</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Structural tokens and delimiting tokens help break down text into meaningful units and signal relationships between these units.
+2. Delimiting tokens, or delimiters, are characters or sequences of characters that mark the beginning or end of a unit of text or data. The primary function of delimiting tokens is to segment text into understandable components like words, phrases, clauses, and sentences, allowing for clear parsing and interpretation.
+3. Structural Tokens (Often called Discourse Markers or Connectives): Structural tokens are words or phrases that signal the logical relationships between different parts of a text, such as sentences or paragraphs.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens are primarily </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>function words</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (such as articles, conjunctions, prepositions, and auxiliary verbs) and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>common noun phrases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> that serve as structural anchors in sentences. These tokens often </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>mark the boundaries of clauses</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>introduce or connect ideas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, and are essential for grammatical cohesion and meaning flow in both narrative and informational contexts."</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Structural anchors: types of words and phrases act like key points or frameworks around which the rest of the sentence is built and organized. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens are often </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>function words</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, conjunctions, prepositions, or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">common short phrases </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">that serve as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>syntactic connectors or modifiers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, as well as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">inflectional </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">or </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">derivational morphemes </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>in various languages. These tokens are crucial for sentence structure, meaning transitions, and grammatical relationships across diverse linguistic contexts."</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Syntactic Connectors: These are words or phrases that link different parts of a sentence or different sentences together e.g. conjunctions, certain function words/common short phrases (Conjunctive Adverbs, Prepositions).
+2. Syntactic Modifiers: These are words or phrases that describe, qualify, or limit the meaning of another word or group of words (the "head") in the sentence. They add more information or detail e.g. Function Words (adjective and adverb), Prepositions, Common Short Phrases, Inflectional or Derivational Morphemes.
+3. Connect: Join different grammatical units to form larger, cohesive structures; Modify: Add detail or specify the meaning of other units within the sentence.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>text segments</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> are typically </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>multi-word phrases or clauses</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> that </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>convey specific actions, states, or relationships</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, often providing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">key contextual or descriptive information </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>within a sentence. These segments frequently include verbs, objects, and modifiers, forming meaningful units that contribute to the overall narrative or informational structure of the text."</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Modifier: adjective and adverb</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted spans often represent </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">multi-word phrases or clauses </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">that function as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>cohesive semantic units</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, such as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>prepositional phrases, idiomatic expressions, or descriptive noun phrases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. These segments frequently provide contextual detail, specify relationships, or add nuance to the main clause, and are typically composed of function words combined with content words to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>form meaningful, context-dependent chunks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens frequently correspond to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>structural elements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in formal or factual writing, such as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>numbers, dates, conjunctions, prepositions, punctuation, and proper nouns</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, which are often used to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>organize, enumerate, or specify information in lists, references, or descriptive passages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The text contains a wide variety of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>conversational and narrative fragments</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, including </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>idiomatic expressions, filler words, discourse markers, and references to people, places, and actions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. There is a frequent use of pronouns, conjunctions, and auxiliary verbs, as well as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>sequences that reflect spoken language patterns such as repetitions, hesitations, and clarifications</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. Many segments highlight</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> the structure of dialogue, question-answer formats, and descriptive or explanatory statements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, often</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> focusing on actions, states, or relationships between entities</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>."</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Discourse markers are words or phrases used to connect and organize ideas in spoken or written language. 
+2. Filler words: These are sounds or words used by speakers to fill silences or pauses in their speech, typically while they are thinking about what to say next, searching for a word, or hesitating. They help the speaker maintain their turn in the conversation without awkward silences.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens are primarily </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>German morphemes, word stems, or inflections</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, often marking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>noun or verb endings, compound word parts, or grammatical function words</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Many are common in German-language text, including noun endings (-en, -heit, -keit, -ung), verb forms (-iert, -te, -en), and connecting words (und, von, in, der, die, das, eine). There is also frequent activation on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>recurring roots in compound nouns and on inflectional suffixes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, reflecting the morphological structure of German."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens are primarily </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">short morphemes, prefixes, or function words </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">in Slavic and related languages, often marking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">grammatical relationships, word formation, or serving as connectors </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>within or between words and phrases."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"The highlighted tokens are primarily</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> German (and some Russian) morphemes, word stems, and inflectional endings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, often marking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>grammatical features such as case, number, tense, or forming compound nouns and verbs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Many are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>parts of longer words or compounds</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, reflecting the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>agglutinative and inflectional nature of German</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, and are often found </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>at the beginning, middle, or end of words</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>."</t>
+    </r>
+  </si>
+  <si>
+    <t>1. An agglutinative language forms words by combining morphemes, which are meaningful word parts, without significantly changing their forms.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens are predominantly </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">morphemes, roots, prefixes, suffixes, or short function words </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">within </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Russian, Bulgarian, and related Slavic texts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. These segments often mark </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>grammatical features, word formation, or serve as connectors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>and are</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> frequently found at the beginning, middle, or end of words</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, reflecting </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>the agglutinative and inflectional nature of these languages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"The highlighted tokens are primarily German</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> function words, verb forms, noun and adjective endings, and common prefixes or suffixes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, often marking grammatical relationships, tense, plurality, or case, as well as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>frequent collocations and set phrases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. These tokens are essential for sentence structure and meaning in German text."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens are primarily </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">morphemes, word stems, suffixes, and grammatical endings in Russian </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">(and some in English), often marking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>case, number, tense, or forming nouns, adjectives, and verbs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. There is a focus on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>functional elements that contribute to word formation, inflection, and syntactic structure</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, as well as on</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> common connective words and phrase boundaries</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens are primarily </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>function words, verb forms, noun and adjective endings, and common collocations in German sentences</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, often marking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>grammatical structure, tense, or case, as well as frequent phrase boundaries and connectors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. These tokens are crucial for sentence construction and meaning in German text."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens are predominantly </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Russian word stems, prefixes, and suffixes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> that form </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>the core of verbs, nouns, and adjectives</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, often marking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>grammatical or semantic roles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> such as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>actions, objects, or qualities</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. These morphemes are crucial for word formation and meaning in Russian, frequently appearing at the beginning or within words to indicate tense, aspect, subject, or object, and are central to the structure and interpretation of Russian sentences."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted spans are predominantly </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>German multi-word expressions, noun or verb phrases, and compound words</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, often marking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>grammatical constructs, inflections, or idiomatic units</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Many are functionally important for sentence structure, such as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>verb-final clauses, participial forms, or noun compounds, and frequently include suffixes or prefixes that signal tense, plurality, or case</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. These patterns reflect the morphological richness and syntactic dependencies characteristic of German text."</t>
+    </r>
+  </si>
+  <si>
+    <t>1. verb-final clause: is a linguistic term referring to a clause where the verb is positioned at the end of the clause, rather than in the middle or at the beginning.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens are predominantly </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>proper nouns, technical terms, and named entities</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">—such as personal names, place names, and institutional or scientific terms—often in multiple languages. These tokens frequently appear </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>in contexts involving formal identification, attribution, or description of people, locations, organizations, or specialized concepts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"The highlighted tokens are predominantly</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> German morphemes, word stems, and grammatical endings, often marking inflections, compounds, or function words.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> These tokens frequently</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> appear at the boundaries of words or phrases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, indicating their importance for understanding German syntax, morphology, and sentence structure."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens are primarily </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>German function words, verb forms, pronouns, and common noun or adjective suffixes, especially those marking person, tense, or plurality</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. There is a strong focus on grammatical structures, such as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>verb conjugations, modal verbs, and case endings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, as well as on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>frequently used collocations and phrasal patterns</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in German sentences."</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Verb conjugation means changing the verb form to reflect tense, person, number, or mood.
+2. Case endings show the grammatical function of nouns, pronouns, and adjectives in a sentence.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens are primarily </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Russian morphemes, roots, and affixes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> that form t</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>he core semantic or grammatical structure of word</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>s, often marking</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> verbs, nouns, or adjectives</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, and are crucial for conveying</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> meaning, tense, aspect, or function</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> within the sentence."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens are predominantly </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Russian morphemes, words, or short phrases</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> that serve as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>key semantic or syntactic units within sentences</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. They include </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>verb roots, noun endings, pronouns, conjunctions, and common collocations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, often marking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>the core meaning, grammatical structure, or transitions in the text</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. The activations focus on elements that define </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>actions, states, relationships, or important contextual information</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, reflecting the building blocks of Russian sentence construction and meaning."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens are predominantly </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Russian morphemes, roots, or affixes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> that form</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> the core semantic or grammatical structure of words</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, often marking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>verbs, adjectives, or nouns</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. These segments frequently appear at the beginning or end of words and are essential for conveying meaning, tense, aspect, or other grammatical features in Russian. The activations </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>focus on these meaningful subword units that are central to word formation and comprehension in the language</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>primarily Russian morphemes, function words, and endings that mark grammatical relationships, verb conjugations, noun/adjective declensions, and common syntactic connectors</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. These tokens are crucial for sentence structure, tense, case, agreement, and linking clauses, reflecting the morphological richness and syntactic dependencies of Russian language."</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Noun and adjective declensions refer to how the endings of nouns and adjectives change based on grammatical case, gender, and number</t>
+  </si>
+  <si>
+    <r>
+      <t>"The highlighted tokens are primarily</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> morphemes, roots, prefixes, and suffixes within Russian words</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, often marking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>word formation, inflection, or derivation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. These segments frequently correspond to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>meaningful subword units</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> that contribute to the grammatical or semantic structure of the word, such as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>case endings, diminutives, verb aspects, or noun/adjective formation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>."</t>
+    </r>
+  </si>
+  <si>
+    <t>1. A diminutive is a modified word form that conveys a smaller size, affection, familiarity, or even disdain depending on the context</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens are predominantly </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Russian (and some other Slavic) word endings, suffixes, and inflections</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> that indicate grammatical case, number, gender, verb tense, or derivational morphology. These endings are crucial for understanding syntactic roles and semantic relationships in the text, as well as for identifying noun, adjective, and verb forms."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"The highlighted tokens are</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> predominantly Russian morphological suffixes, prepositions, conjunctions, and noun/adjective endings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> that indicate grammatical relationships, case, number, gender, and aspect. These elements are essential for syntactic structure and meaning in Russian, often marking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>possession, agency, time, and other core grammatical functions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"The important tokens are predominantly</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Russian morphemes, roots, and affixes that form the core semantic or grammatical structure of words</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, often marking </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>noun, verb, or adjective stems, as well as common derivational and inflectional endings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. These tokens frequently appear at the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>beginning or within the main body of words</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, highlighting the morphological building blocks essential for meaning and word formation in Russian text."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"The highlighted tokens are predominantly</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> German suffixes and word endings that form nouns, adjectives, and participles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, often indicating grammatical features such as case, number, gender, or degree, as well as forming</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> compound words and inflections</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"The highlighted tokens are predominantly</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Russian morphemes, roots, and affixes that form the core semantic or grammatical structure of words</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. These include verb and noun roots, derivational and inflectional suffixes, and key word segments that contribute to meaning, tense, aspect, or case. The pattern reflects a focus on the internal morphological structure of Russian words, emphasizing the parts that carry essential lexical or grammatical information."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens are primarily </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>German morphemes, function words, and common suffixes or inflections</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, as well as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>high-frequency connectors and pronouns</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. These include verb and noun endings, conjunctions, prepositions, and pronouns, which are essential for sentence structure and meaning in German text. The activations also emphasize </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>recurring grammatical patterns, such as subordinate clause markers, verb conjugations, and noun/adjective endings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, reflecting the importance of syntactic and morphological elements in German language processing."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"The highlighted tokens are predominantly</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> German morphemes, function words, and common suffixes or inflections</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, often marking</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> verb forms, noun endings, or grammatical particles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. These tokens frequently appear at the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> boundaries of words or as part of compound constructions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, reflecting the morphological richness and syntactic structure of German text."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens are predominantly </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>German function words, inflectional endings, and common noun or adjective suffixes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, reflecting grammatical structure such as articles, pronouns, prepositions, conjunctions, and case or number markers essential for sentence construction and meaning."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"The highlighted tokens are primarily </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Russian morphemes, roots, and affixes that form the semantic and grammatical core of words, often marking key concepts, actions, or relationships within sentences</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>. These include noun, verb, and adjective roots, as well as frequent derivational and inflectional suffixes, reflecting the morphological structure and meaning-bearing elements of the language."</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -501,7 +2575,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -524,11 +2598,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -547,6 +2632,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -852,10 +2952,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -865,94 +2965,110 @@
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="53" style="1" customWidth="1"/>
     <col min="5" max="5" width="47.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="120.33203125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="55.2" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="5">
         <v>93066</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>11</v>
+        <v>120</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="5">
         <v>128132</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>12</v>
+        <v>122</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="5">
         <v>14207</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>13</v>
+        <v>124</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="5">
         <v>34138</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>14</v>
+        <v>126</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -963,30 +3079,30 @@
         <v>12333</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="5">
         <v>123973</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
@@ -997,13 +3113,13 @@
         <v>19293</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
@@ -1014,44 +3130,47 @@
         <v>37895</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="69" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="5">
         <v>5889</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>19</v>
+        <v>129</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="138" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="138" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="5">
         <v>67343</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>20</v>
+        <v>130</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1062,10 +3181,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1075,26 +3194,30 @@
     <col min="3" max="3" width="12.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="53" style="1" customWidth="1"/>
     <col min="5" max="5" width="47.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="64.109375" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>146</v>
+        <v>117</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="69" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="69" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1105,13 +3228,13 @@
         <v>123218</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="55.2" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -1125,10 +3248,10 @@
         <v>11</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="41.4" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -1139,15 +3262,15 @@
         <v>64723</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>142</v>
+        <v>113</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="69" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="69" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>8</v>
@@ -1156,15 +3279,15 @@
         <v>32578</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>10</v>
@@ -1173,13 +3296,13 @@
         <v>84692</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
@@ -1190,66 +3313,66 @@
         <v>14207</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="124.2" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>38</v>
+      <c r="B8" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C8" s="5">
         <v>56064</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>49</v>
+        <v>132</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C9" s="5">
         <v>100192</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C10" s="5">
         <v>105874</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>8</v>
@@ -1258,64 +3381,64 @@
         <v>98476</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C12" s="5">
         <v>120200</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="69" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="69" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C13" s="5">
         <v>4518</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="55.2" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="69" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>42</v>
+      <c r="B14" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C14" s="5">
         <v>48343</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>55</v>
+        <v>133</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>3</v>
       </c>
@@ -1326,13 +3449,13 @@
         <v>12333</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>3</v>
       </c>
@@ -1343,98 +3466,101 @@
         <v>30265</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>38</v>
+      <c r="B17" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C17" s="5">
         <v>31366</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>57</v>
+        <v>134</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="55.2" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C18" s="5">
         <v>49501</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>42</v>
+        <v>28</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C19" s="5">
         <v>121507</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>59</v>
+        <v>136</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="69" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="69" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C20" s="5">
         <v>68498</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C21" s="5">
         <v>70835</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>4</v>
       </c>
@@ -1445,66 +3571,66 @@
         <v>123973</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>38</v>
+      <c r="B23" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C23" s="5">
         <v>79729</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>62</v>
+        <v>137</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>42</v>
+      <c r="B24" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C24" s="5">
         <v>109317</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>63</v>
+        <v>138</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C25" s="5">
         <v>9083</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>64</v>
+        <v>139</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>9</v>
@@ -1513,32 +3639,32 @@
         <v>77250</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>42</v>
+        <v>30</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C27" s="5">
         <v>59767</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>66</v>
+        <v>140</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>8</v>
@@ -1547,15 +3673,15 @@
         <v>41383</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>8</v>
@@ -1564,47 +3690,50 @@
         <v>43549</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="124.2" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>38</v>
+        <v>31</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C30" s="5">
         <v>44371</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>42</v>
+        <v>31</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C31" s="5">
         <v>56594</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>70</v>
+        <v>143</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>5</v>
       </c>
@@ -1615,115 +3744,118 @@
         <v>52975</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>38</v>
+      <c r="B33" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C33" s="5">
         <v>27401</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>38</v>
+      <c r="B34" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C34" s="5">
         <v>52681</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>73</v>
+        <v>145</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="69" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="69" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C35" s="5">
         <v>63085</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C36" s="5">
         <v>102511</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="138" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="138" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>42</v>
+      <c r="B37" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C37" s="5">
         <v>8452</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>76</v>
+        <v>148</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="69" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="69" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>42</v>
+      <c r="B38" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C38" s="5">
         <v>74675</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>77</v>
+        <v>147</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>5</v>
       </c>
@@ -1734,15 +3866,15 @@
         <v>37895</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>8</v>
@@ -1751,66 +3883,69 @@
         <v>16648</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="69" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="69" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C41" s="5">
         <v>13954</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="124.2" x14ac:dyDescent="0.3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="124.2" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>42</v>
+        <v>32</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C42" s="5">
         <v>31110</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>80</v>
+        <v>149</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>42</v>
+        <v>32</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C43" s="5">
         <v>48228</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>81</v>
+        <v>150</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>8</v>
@@ -1819,117 +3954,120 @@
         <v>91108</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C45" s="5">
         <v>29244</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>83</v>
+        <v>152</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C46" s="5">
         <v>40052</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>84</v>
+        <v>154</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C47" s="5">
         <v>97322</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>85</v>
+        <v>155</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>42</v>
+        <v>33</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C48" s="5">
         <v>115738</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>86</v>
+        <v>156</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>133</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C49" s="5">
         <v>53088</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>134</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="C50" s="5">
         <v>40808</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>8</v>
@@ -1938,78 +4076,78 @@
         <v>14651</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C52" s="5">
         <v>312</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>90</v>
+        <v>157</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C53" s="5">
         <v>27401</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C54" s="5">
         <v>108954</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>138</v>
+        <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>42</v>
+        <v>34</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C55" s="5">
         <v>44860</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="69" x14ac:dyDescent="0.3">
@@ -2023,78 +4161,78 @@
         <v>5889</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>139</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="138" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>38</v>
+      <c r="B57" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C57" s="5">
         <v>17109</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>94</v>
+        <v>159</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>38</v>
+      <c r="B58" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C58" s="5">
         <v>75403</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>95</v>
+        <v>160</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="69" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="82.8" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>38</v>
+      <c r="B59" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C59" s="5">
         <v>130833</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>96</v>
+        <v>161</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>140</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>42</v>
+      <c r="B60" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C60" s="5">
         <v>56964</v>
       </c>
       <c r="D60" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E60" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="138" x14ac:dyDescent="0.3">
@@ -2102,16 +4240,16 @@
         <v>6</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C61" s="5">
         <v>66481</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>